<commit_message>
Added New test case and Added Logger login
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sopan.sagorkar\eclipse-workspace\seleniumframework\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D4B77F8-51BE-45EF-9B34-E47AB6302F28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAC0DDA9-8043-4F3D-992E-BF56F66BF024}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{38366C3F-1F87-4778-8E3C-AE3BD4D4965C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{38366C3F-1F87-4778-8E3C-AE3BD4D4965C}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
-    <sheet name="Register" sheetId="2" r:id="rId2"/>
+    <sheet name="SearchHotel" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Username</t>
   </si>
@@ -46,13 +46,37 @@
   </si>
   <si>
     <t>demouser</t>
+  </si>
+  <si>
+    <t>Destination</t>
+  </si>
+  <si>
+    <t>Checkin</t>
+  </si>
+  <si>
+    <t>Checkout</t>
+  </si>
+  <si>
+    <t>Adults</t>
+  </si>
+  <si>
+    <t>Child</t>
+  </si>
+  <si>
+    <t>Indore</t>
+  </si>
+  <si>
+    <t>10/7/2021</t>
+  </si>
+  <si>
+    <t>11/7/2021</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -66,6 +90,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -75,7 +107,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -83,13 +115,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -406,8 +458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96A760AF-B4CB-43C7-89E0-161BE794EF90}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -417,10 +469,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
@@ -440,12 +492,53 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2299026-0FB5-432D-A3AE-CF5EFF53D8DA}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="3">
+        <v>2</v>
+      </c>
+      <c r="E2" s="3">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>